<commit_message>
added support for nil columns
</commit_message>
<xml_diff>
--- a/specs/test.xlsx
+++ b/specs/test.xlsx
@@ -15,9 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>teststring</t>
+  </si>
+  <si>
+    <t>dataa1</t>
+  </si>
+  <si>
+    <t>datac1</t>
+  </si>
+  <si>
+    <t>datad1</t>
   </si>
 </sst>
 </file>
@@ -124,10 +133,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:KN117"/>
+  <dimension ref="A1:KN118"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A94" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="F106" activeCellId="0" pane="topLeft" sqref="F106"/>
+      <selection activeCell="A104" activeCellId="0" pane="topLeft" sqref="A104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1635,6 +1644,17 @@
         <v>41091.8881134259</v>
       </c>
     </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="118">
+      <c r="A118" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C118" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D118" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>